<commit_message>
Updates to my normal backlogs.  Ahhh!  How nice to be using Notepad++, my friends!
</commit_message>
<xml_diff>
--- a/Dev Notes/Master Backlog.xlsx
+++ b/Dev Notes/Master Backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6885" tabRatio="829"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="130">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -342,9 +342,6 @@
     <t>New Honda Problem List</t>
   </si>
   <si>
-    <t>Listen to Wapnik's Intro</t>
-  </si>
-  <si>
     <t>De-commission / replace Big Blue / Get a Monitor</t>
   </si>
   <si>
@@ -390,22 +387,31 @@
     <t>Honda Accord Jack - Salvage Yards - 630-860-2000 =&gt; go get it!</t>
   </si>
   <si>
-    <t>Configure Automatic Backups / Storage Architecture</t>
-  </si>
-  <si>
-    <t>Get More T-Shirts &amp; Fighter Shorts &amp; Borns Shoes</t>
-  </si>
-  <si>
-    <t>New Gi (PLEASE)</t>
-  </si>
-  <si>
     <t>ProjectLocker - +1</t>
   </si>
   <si>
-    <t>Pleiades (Git Tools, MVC Postback)</t>
-  </si>
-  <si>
     <t>Buy Resharper - for productivity</t>
+  </si>
+  <si>
+    <t>Pleiades (Product Management, Git Tools, MVC Postback)</t>
+  </si>
+  <si>
+    <t>http://naturalsoapboutique.com/natural-hand-made-soap - for Mom</t>
+  </si>
+  <si>
+    <t>New Gi (PLEASE) + Fight Shorts</t>
+  </si>
+  <si>
+    <t>Get More T-Shirts &amp; Borns Shoes http://www.aeropostale.com</t>
+  </si>
+  <si>
+    <t>PLEASE COME UP WITH A BUDGET!</t>
+  </si>
+  <si>
+    <t>Honda Brake Job!</t>
+  </si>
+  <si>
+    <t>Backup Before Vaca / Configure Automatic Backups / Storage Architecture</t>
   </si>
 </sst>
 </file>
@@ -559,8 +565,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -858,15 +864,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="64.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" style="7" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
@@ -888,45 +894,45 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B5" s="10" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="10" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>120</v>
+      <c r="A9" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="4" t="s">
-        <v>122</v>
+      <c r="A10" s="24" t="s">
+        <v>121</v>
       </c>
       <c r="B10" s="24" t="s">
         <v>0</v>
@@ -934,7 +940,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>101</v>
@@ -947,69 +953,88 @@
       <c r="B13"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="25" t="s">
         <v>124</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>0</v>
+        <v>127</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="25" t="s">
-        <v>121</v>
+      <c r="A16" s="24" t="s">
+        <v>128</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="25" t="s">
-        <v>118</v>
+      <c r="A17" s="24" t="s">
+        <v>120</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="3" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="3" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="23" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="18" t="s">
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B24" s="22" t="s">
         <v>100</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A14" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1033,37 +1058,37 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1093,7 +1118,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>27</v>
@@ -1128,7 +1153,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:2">

</xml_diff>

<commit_message>
Massive, massive changes to refactor for the Pleiades Framework and the overhaul of the Security model to use Code First.
</commit_message>
<xml_diff>
--- a/Dev Notes/Master Backlog.xlsx
+++ b/Dev Notes/Master Backlog.xlsx
@@ -18,11 +18,12 @@
     <sheet name="Hosts" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="127">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -111,9 +112,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>Fun Stuff</t>
-  </si>
-  <si>
     <t>Essential</t>
   </si>
   <si>
@@ -342,9 +340,6 @@
     <t>New Honda Problem List</t>
   </si>
   <si>
-    <t>De-commission / replace Big Blue / Get a Monitor</t>
-  </si>
-  <si>
     <t>Read the ACIM Text</t>
   </si>
   <si>
@@ -381,37 +376,34 @@
     <t>Get some Moby from somewhere online</t>
   </si>
   <si>
-    <t>TO DO</t>
-  </si>
-  <si>
     <t>Honda Accord Jack - Salvage Yards - 630-860-2000 =&gt; go get it!</t>
   </si>
   <si>
-    <t>ProjectLocker - +1</t>
-  </si>
-  <si>
     <t>Buy Resharper - for productivity</t>
   </si>
   <si>
-    <t>Pleiades (Product Management, Git Tools, MVC Postback)</t>
-  </si>
-  <si>
     <t>http://naturalsoapboutique.com/natural-hand-made-soap - for Mom</t>
   </si>
   <si>
-    <t>New Gi (PLEASE) + Fight Shorts</t>
-  </si>
-  <si>
     <t>Get More T-Shirts &amp; Borns Shoes http://www.aeropostale.com</t>
   </si>
   <si>
     <t>PLEASE COME UP WITH A BUDGET!</t>
   </si>
   <si>
-    <t>Honda Brake Job!</t>
-  </si>
-  <si>
-    <t>Backup Before Vaca / Configure Automatic Backups / Storage Architecture</t>
+    <t>Configure Automatic Backups / Storage Architecture</t>
+  </si>
+  <si>
+    <t>Other Stuff</t>
+  </si>
+  <si>
+    <t>Get a Monitor / De-commission / Replace Big Blue</t>
+  </si>
+  <si>
+    <t>RETURN GI</t>
+  </si>
+  <si>
+    <t>Pleiades (Product Management, Git Tools, MVC)</t>
   </si>
 </sst>
 </file>
@@ -529,7 +521,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -561,12 +553,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -864,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -888,13 +883,13 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>0</v>
@@ -908,7 +903,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="10" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>0</v>
@@ -916,122 +911,106 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>101</v>
+        <v>124</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="24" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="24" t="s">
+      <c r="B13" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="25" t="s">
-        <v>124</v>
-      </c>
       <c r="B14" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>101</v>
+      <c r="A15" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="24" t="s">
+      <c r="A16" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
-        <v>29</v>
+      <c r="B20" s="25" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>101</v>
+      <c r="A21" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="B24" s="22" t="s">
+      <c r="A22" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A14" r:id="rId1"/>
+    <hyperlink ref="A13" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1053,42 +1032,42 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
       <c r="A1" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1118,7 +1097,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>27</v>
@@ -1129,7 +1108,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1137,7 +1116,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1153,7 +1132,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1169,7 +1148,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1194,7 +1173,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="23.25">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -1204,7 +1183,7 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -1214,12 +1193,12 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -1249,39 +1228,39 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25">
       <c r="A1" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1309,43 +1288,43 @@
   <sheetData>
     <row r="1" spans="1:7" ht="23.25">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1353,17 +1332,17 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1383,7 +1362,7 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -1396,7 +1375,7 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:1">
@@ -1431,7 +1410,7 @@
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1456,7 +1435,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25">
       <c r="A1" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1464,105 +1443,105 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1592,28 +1571,28 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25">
       <c r="A1" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>3</v>
@@ -1621,7 +1600,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>1</v>
@@ -1629,7 +1608,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>2</v>
@@ -1637,17 +1616,17 @@
     </row>
     <row r="8" spans="1:2">
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1670,42 +1649,42 @@
   <sheetData>
     <row r="1" spans="1:1" ht="23.25">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest revision to separate out the Domain Authorization logic to separate assembly
</commit_message>
<xml_diff>
--- a/Dev Notes/Master Backlog.xlsx
+++ b/Dev Notes/Master Backlog.xlsx
@@ -18,12 +18,11 @@
     <sheet name="Hosts" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="126">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -373,18 +372,12 @@
     <t>Fix Honda Powerlock</t>
   </si>
   <si>
-    <t>Get some Moby from somewhere online</t>
-  </si>
-  <si>
     <t>Honda Accord Jack - Salvage Yards - 630-860-2000 =&gt; go get it!</t>
   </si>
   <si>
     <t>Buy Resharper - for productivity</t>
   </si>
   <si>
-    <t>http://naturalsoapboutique.com/natural-hand-made-soap - for Mom</t>
-  </si>
-  <si>
     <t>Get More T-Shirts &amp; Borns Shoes http://www.aeropostale.com</t>
   </si>
   <si>
@@ -404,6 +397,9 @@
   </si>
   <si>
     <t>Pleiades (Product Management, Git Tools, MVC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moby, Bon Iver, </t>
   </si>
 </sst>
 </file>
@@ -521,7 +517,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -554,7 +550,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -859,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -903,7 +898,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>0</v>
@@ -911,15 +906,15 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B8" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>100</v>
@@ -927,9 +922,9 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>100</v>
       </c>
     </row>
@@ -940,7 +935,7 @@
       <c r="B12"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="10" t="s">
         <v>119</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -948,72 +943,61 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>99</v>
+      <c r="A14" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B15" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="B16" s="25" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" s="24" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="10" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="23" t="s">
-        <v>120</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="B21" s="26" t="s">
+      <c r="A21" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>100</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Completion of refactoring Identity Unit Tests.  Also: stubbed out MembershipProvider Unit Tests and moved integration stuff in Framework.IntegrationTests
</commit_message>
<xml_diff>
--- a/Dev Notes/Master Backlog.xlsx
+++ b/Dev Notes/Master Backlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="127">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -378,12 +378,6 @@
     <t>Buy Resharper - for productivity</t>
   </si>
   <si>
-    <t>Get More T-Shirts &amp; Borns Shoes http://www.aeropostale.com</t>
-  </si>
-  <si>
-    <t>PLEASE COME UP WITH A BUDGET!</t>
-  </si>
-  <si>
     <t>Configure Automatic Backups / Storage Architecture</t>
   </si>
   <si>
@@ -396,10 +390,19 @@
     <t>RETURN GI</t>
   </si>
   <si>
-    <t>Pleiades (Product Management, Git Tools, MVC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moby, Bon Iver, </t>
+    <t>Pleiades (Refactor C#, Product Management, Git Tools, MVC)</t>
+  </si>
+  <si>
+    <t>Get More T-Shirts - see links + http://www.aeropostale.com</t>
+  </si>
+  <si>
+    <t>Moby, Bon Iver, Chicago Mix Tape, etc.</t>
+  </si>
+  <si>
+    <t>PLEASE COME UP WITH A BUDGET! &amp; LOG INTO PAYROLL WEBSITE</t>
+  </si>
+  <si>
+    <t>Goto Fleetfeet</t>
   </si>
 </sst>
 </file>
@@ -517,7 +520,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -556,7 +559,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -854,7 +858,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
@@ -898,23 +902,23 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" s="26" t="s">
+      <c r="A8" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>100</v>
@@ -922,9 +926,9 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>100</v>
       </c>
     </row>
@@ -936,7 +940,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="10" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>99</v>
@@ -960,38 +964,46 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>100</v>
+      <c r="A19" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="24" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B22" s="22" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished the Great Refactoring #1 of Integration Tests
</commit_message>
<xml_diff>
--- a/Dev Notes/Master Backlog.xlsx
+++ b/Dev Notes/Master Backlog.xlsx
@@ -387,9 +387,6 @@
     <t>Get a Monitor / De-commission / Replace Big Blue</t>
   </si>
   <si>
-    <t>RETURN GI</t>
-  </si>
-  <si>
     <t>Pleiades (Refactor C#, Product Management, Git Tools, MVC)</t>
   </si>
   <si>
@@ -402,7 +399,10 @@
     <t>PLEASE COME UP WITH A BUDGET! &amp; LOG INTO PAYROLL WEBSITE</t>
   </si>
   <si>
-    <t>Goto Fleetfeet</t>
+    <t>Replace cooling fan and heat sink</t>
+  </si>
+  <si>
+    <t>Gi + Gloves</t>
   </si>
 </sst>
 </file>
@@ -861,7 +861,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -902,77 +902,77 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B9" s="27" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B12"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="23" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B15" s="24" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -985,7 +985,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>100</v>
@@ -993,7 +993,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
Working on wiring refactored AggregateUser together.  Broken build at this stage.
</commit_message>
<xml_diff>
--- a/Dev Notes/Master Backlog.xlsx
+++ b/Dev Notes/Master Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="75">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -201,9 +201,6 @@
     <t>Feb 2013?</t>
   </si>
   <si>
-    <t>Fix Honda Powerlock</t>
-  </si>
-  <si>
     <t>Honda Accord Jack - Salvage Yards - 630-860-2000 =&gt; go get it!</t>
   </si>
   <si>
@@ -222,22 +219,31 @@
     <t>Pleiades (Refactor C#, Product Management, Git Tools, MVC)</t>
   </si>
   <si>
-    <t>Get More T-Shirts - see links + http://www.aeropostale.com</t>
-  </si>
-  <si>
-    <t>Moby, Bon Iver, Chicago Mix Tape, etc.</t>
-  </si>
-  <si>
-    <t>PLEASE COME UP WITH A BUDGET! &amp; LOG INTO PAYROLL WEBSITE</t>
-  </si>
-  <si>
-    <t>Replace cooling fan and heat sink</t>
-  </si>
-  <si>
-    <t>Gi + Gloves</t>
-  </si>
-  <si>
-    <t>Pipe</t>
+    <t>Get More T-Shirts - see links in browser window</t>
+  </si>
+  <si>
+    <t>Moby, Bon Iver, Arcade Fire, Group Love, Chicago Mix Tape, etc.</t>
+  </si>
+  <si>
+    <t>Replace cooling fan and heat sink on Yipman</t>
+  </si>
+  <si>
+    <t>Pipe/Rattle</t>
+  </si>
+  <si>
+    <t>Clean Honda</t>
+  </si>
+  <si>
+    <t>Buy a Gi</t>
+  </si>
+  <si>
+    <t>Hardware Store</t>
+  </si>
+  <si>
+    <t>House Hunting Backlog</t>
+  </si>
+  <si>
+    <t>Login to Payroll Website, Do Collections</t>
   </si>
 </sst>
 </file>
@@ -358,8 +364,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -656,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -700,108 +706,124 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>0</v>
+      <c r="A8" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13"/>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="9" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="17" t="s">
-        <v>61</v>
+      <c r="A15" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="17" t="s">
-        <v>60</v>
+      <c r="A16" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="2" t="s">
-        <v>64</v>
+    <row r="17" spans="1:2">
+      <c r="A17" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B21" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B23" s="19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="15" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B24" s="16" t="s">
         <v>45</v>
       </c>
     </row>
@@ -896,7 +918,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -946,7 +968,7 @@
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the MVC Routing Tests.  w00t!
</commit_message>
<xml_diff>
--- a/Dev Notes/Master Backlog.xlsx
+++ b/Dev Notes/Master Backlog.xlsx
@@ -13,13 +13,14 @@
     <sheet name="Stuff To Buy" sheetId="6" r:id="rId4"/>
     <sheet name="Services, Markets &amp; Ideas" sheetId="13" r:id="rId5"/>
     <sheet name="Hosts" sheetId="9" r:id="rId6"/>
+    <sheet name="SCIGON Payroll Summary" sheetId="15" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -207,43 +208,70 @@
     <t>Buy Resharper - for productivity</t>
   </si>
   <si>
-    <t>Configure Automatic Backups / Storage Architecture</t>
-  </si>
-  <si>
     <t>Other Stuff</t>
   </si>
   <si>
-    <t>Get a Monitor / De-commission / Replace Big Blue</t>
-  </si>
-  <si>
-    <t>Pleiades (Refactor C#, Product Management, Git Tools, MVC)</t>
-  </si>
-  <si>
     <t>Get More T-Shirts - see links in browser window</t>
   </si>
   <si>
     <t>Moby, Bon Iver, Arcade Fire, Group Love, Chicago Mix Tape, etc.</t>
   </si>
   <si>
-    <t>Replace cooling fan and heat sink on Yipman</t>
-  </si>
-  <si>
     <t>Pipe/Rattle</t>
   </si>
   <si>
-    <t>Clean Honda</t>
-  </si>
-  <si>
-    <t>Buy a Gi</t>
-  </si>
-  <si>
     <t>Hardware Store</t>
   </si>
   <si>
     <t>House Hunting Backlog</t>
   </si>
   <si>
-    <t>Login to Payroll Website, Do Collections</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Storage Architecture for Media</t>
+  </si>
+  <si>
+    <t>Configure Automatic Backups</t>
+  </si>
+  <si>
+    <t>Find Invoicing Software</t>
+  </si>
+  <si>
+    <t>Bike Store + Bike Rack</t>
+  </si>
+  <si>
+    <t>Bike Handlebars</t>
+  </si>
+  <si>
+    <t>WAITING ON MARIAS CARD</t>
+  </si>
+  <si>
+    <t>Pleiades (MVC + C# + Git + JavaScript + Azure)</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>De-commission Big Blue</t>
+  </si>
+  <si>
+    <t>SUNDAY</t>
+  </si>
+  <si>
+    <t>SATURDAY</t>
+  </si>
+  <si>
+    <t>CALL THAT BIKESHOP</t>
+  </si>
+  <si>
+    <t>Call Tax Accountants</t>
   </si>
 </sst>
 </file>
@@ -276,20 +304,20 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +348,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -333,41 +373,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,22 +707,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="67.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="72.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" ht="26.25">
+      <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -691,10 +736,10 @@
       <c r="B3"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="19" t="s">
         <v>0</v>
       </c>
     </row>
@@ -705,125 +750,138 @@
       <c r="B6"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B9" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>45</v>
+      <c r="A15" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>45</v>
+      <c r="A16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="21" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="18" t="s">
+      <c r="B23" s="23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="19" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="15" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B25" s="22" t="s">
         <v>45</v>
       </c>
     </row>
@@ -844,7 +902,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25">
@@ -853,10 +911,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -864,7 +922,7 @@
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -872,7 +930,7 @@
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -880,7 +938,7 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -888,7 +946,7 @@
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>59</v>
       </c>
     </row>
@@ -896,7 +954,7 @@
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -904,7 +962,7 @@
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>47</v>
       </c>
     </row>
@@ -927,7 +985,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>49</v>
       </c>
     </row>
@@ -968,7 +1026,7 @@
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1018,7 +1076,7 @@
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1048,7 +1106,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1058,7 +1116,7 @@
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1179,4 +1237,167 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3">
+      <c r="A3" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="17">
+        <v>40931</v>
+      </c>
+      <c r="B4" s="17">
+        <v>40944</v>
+      </c>
+      <c r="C4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="17">
+        <v>40945</v>
+      </c>
+      <c r="B5" s="17">
+        <v>40958</v>
+      </c>
+      <c r="C5">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="17">
+        <v>40959</v>
+      </c>
+      <c r="B6" s="17">
+        <v>40972</v>
+      </c>
+      <c r="C6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="17">
+        <v>40973</v>
+      </c>
+      <c r="B7" s="17">
+        <v>40986</v>
+      </c>
+      <c r="C7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="17">
+        <v>40987</v>
+      </c>
+      <c r="B8" s="17">
+        <v>41000</v>
+      </c>
+      <c r="C8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="17">
+        <v>41001</v>
+      </c>
+      <c r="B9" s="17">
+        <v>41014</v>
+      </c>
+      <c r="C9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="17">
+        <v>41015</v>
+      </c>
+      <c r="B10" s="17">
+        <v>41028</v>
+      </c>
+      <c r="C10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="17">
+        <v>41029</v>
+      </c>
+      <c r="B11" s="17">
+        <v>41042</v>
+      </c>
+      <c r="C11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="17">
+        <v>41043</v>
+      </c>
+      <c r="B12" s="17">
+        <v>41056</v>
+      </c>
+      <c r="C12">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="17">
+        <v>41057</v>
+      </c>
+      <c r="B13" s="17">
+        <v>41070</v>
+      </c>
+      <c r="C13">
+        <v>74.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="17">
+        <v>41071</v>
+      </c>
+      <c r="B14" s="17">
+        <v>41084</v>
+      </c>
+      <c r="C14">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="17">
+        <v>41085</v>
+      </c>
+      <c r="B15" s="17">
+        <v>41098</v>
+      </c>
+      <c r="C15">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Another massive work session - moving logic from Controller into Execution framework.
</commit_message>
<xml_diff>
--- a/Dev Notes/Master Backlog.xlsx
+++ b/Dev Notes/Master Backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Random Stuff</t>
   </si>
   <si>
-    <t>ON QUEUE</t>
-  </si>
-  <si>
     <t>TODO</t>
   </si>
   <si>
@@ -205,24 +202,15 @@
     <t>Honda Accord Jack - Salvage Yards - 630-860-2000 =&gt; go get it!</t>
   </si>
   <si>
-    <t>Buy Resharper - for productivity</t>
-  </si>
-  <si>
     <t>Other Stuff</t>
   </si>
   <si>
-    <t>Get More T-Shirts - see links in browser window</t>
-  </si>
-  <si>
     <t>Moby, Bon Iver, Arcade Fire, Group Love, Chicago Mix Tape, etc.</t>
   </si>
   <si>
     <t>Pipe/Rattle</t>
   </si>
   <si>
-    <t>Hardware Store</t>
-  </si>
-  <si>
     <t>House Hunting Backlog</t>
   </si>
   <si>
@@ -238,15 +226,9 @@
     <t>Find Invoicing Software</t>
   </si>
   <si>
-    <t>Bike Store + Bike Rack</t>
-  </si>
-  <si>
     <t>Bike Handlebars</t>
   </si>
   <si>
-    <t>WAITING ON MARIAS CARD</t>
-  </si>
-  <si>
     <t>Pleiades (MVC + C# + Git + JavaScript + Azure)</t>
   </si>
   <si>
@@ -262,16 +244,31 @@
     <t>De-commission Big Blue</t>
   </si>
   <si>
-    <t>SUNDAY</t>
-  </si>
-  <si>
     <t>SATURDAY</t>
   </si>
   <si>
-    <t>CALL THAT BIKESHOP</t>
-  </si>
-  <si>
     <t>Call Tax Accountants</t>
+  </si>
+  <si>
+    <t>MONDAY</t>
+  </si>
+  <si>
+    <t>CALL GUY BACK</t>
+  </si>
+  <si>
+    <t>Fix the Bike Store + Lights</t>
+  </si>
+  <si>
+    <t>Buy Student Edition Photoshop</t>
+  </si>
+  <si>
+    <t>Buy Resharper</t>
+  </si>
+  <si>
+    <t>Figure out Bike Rack</t>
+  </si>
+  <si>
+    <t>T-Shirts, Jeans, Jack Purcells - see links in browser window</t>
   </si>
 </sst>
 </file>
@@ -373,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -393,9 +390,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -707,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -722,7 +716,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="26.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>4</v>
       </c>
     </row>
@@ -736,10 +730,10 @@
       <c r="B3"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>0</v>
       </c>
     </row>
@@ -750,139 +744,147 @@
       <c r="B6"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>81</v>
+      <c r="B15" s="18" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>45</v>
+      <c r="A17" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>45</v>
+      <c r="A20" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>45</v>
+      <c r="A21" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="18" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>45</v>
+      <c r="B23" s="19" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>45</v>
+      <c r="A24" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>45</v>
+      <c r="A25" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -912,7 +914,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>17</v>
@@ -923,7 +925,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -931,7 +933,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -947,7 +949,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -963,7 +965,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -986,47 +988,47 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
       <c r="A1" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1255,21 +1257,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
-      <c r="A3" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>76</v>
+      <c r="A3" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="17">
+      <c r="A4" s="16">
         <v>40931</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>40944</v>
       </c>
       <c r="C4">
@@ -1277,10 +1279,10 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="17">
+      <c r="A5" s="16">
         <v>40945</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="16">
         <v>40958</v>
       </c>
       <c r="C5">
@@ -1288,10 +1290,10 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="17">
+      <c r="A6" s="16">
         <v>40959</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="16">
         <v>40972</v>
       </c>
       <c r="C6">
@@ -1299,10 +1301,10 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="17">
+      <c r="A7" s="16">
         <v>40973</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>40986</v>
       </c>
       <c r="C7">
@@ -1310,10 +1312,10 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="17">
+      <c r="A8" s="16">
         <v>40987</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="16">
         <v>41000</v>
       </c>
       <c r="C8">
@@ -1321,10 +1323,10 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="17">
+      <c r="A9" s="16">
         <v>41001</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <v>41014</v>
       </c>
       <c r="C9">
@@ -1332,10 +1334,10 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="17">
+      <c r="A10" s="16">
         <v>41015</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="16">
         <v>41028</v>
       </c>
       <c r="C10">
@@ -1343,10 +1345,10 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="17">
+      <c r="A11" s="16">
         <v>41029</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>41042</v>
       </c>
       <c r="C11">
@@ -1354,10 +1356,10 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="17">
+      <c r="A12" s="16">
         <v>41043</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="16">
         <v>41056</v>
       </c>
       <c r="C12">
@@ -1365,10 +1367,10 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="17">
+      <c r="A13" s="16">
         <v>41057</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="16">
         <v>41070</v>
       </c>
       <c r="C13">
@@ -1376,10 +1378,10 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="17">
+      <c r="A14" s="16">
         <v>41071</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="16">
         <v>41084</v>
       </c>
       <c r="C14">
@@ -1387,10 +1389,10 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="17">
+      <c r="A15" s="16">
         <v>41085</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="16">
         <v>41098</v>
       </c>
       <c r="C15">

</xml_diff>

<commit_message>
Moved Commerce.Web to Framework.Web
</commit_message>
<xml_diff>
--- a/Dev Notes/Master Backlog.xlsx
+++ b/Dev Notes/Master Backlog.xlsx
@@ -4,23 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6885" tabRatio="829"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6885" tabRatio="829" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Generic Backlog" sheetId="2" r:id="rId1"/>
-    <sheet name="Try, Do, Explore" sheetId="8" r:id="rId2"/>
-    <sheet name="New Honda Problems" sheetId="14" r:id="rId3"/>
-    <sheet name="Stuff To Buy" sheetId="6" r:id="rId4"/>
-    <sheet name="Services, Markets &amp; Ideas" sheetId="13" r:id="rId5"/>
-    <sheet name="Hosts" sheetId="9" r:id="rId6"/>
-    <sheet name="SCIGON Payroll Summary" sheetId="15" r:id="rId7"/>
+    <sheet name="SCIGON Payroll Summary" sheetId="15" r:id="rId2"/>
+    <sheet name="Try, Do, Explore" sheetId="8" r:id="rId3"/>
+    <sheet name="New Honda Problems" sheetId="14" r:id="rId4"/>
+    <sheet name="Stuff To Buy" sheetId="6" r:id="rId5"/>
+    <sheet name="Services, Markets &amp; Ideas" sheetId="13" r:id="rId6"/>
+    <sheet name="Hosts" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -244,31 +244,22 @@
     <t>De-commission Big Blue</t>
   </si>
   <si>
-    <t>SATURDAY</t>
-  </si>
-  <si>
     <t>Call Tax Accountants</t>
   </si>
   <si>
-    <t>MONDAY</t>
-  </si>
-  <si>
     <t>CALL GUY BACK</t>
   </si>
   <si>
-    <t>Fix the Bike Store + Lights</t>
-  </si>
-  <si>
     <t>Buy Student Edition Photoshop</t>
   </si>
   <si>
     <t>Buy Resharper</t>
   </si>
   <si>
-    <t>Figure out Bike Rack</t>
-  </si>
-  <si>
-    <t>T-Shirts, Jeans, Jack Purcells - see links in browser window</t>
+    <t>T-Shirts, Jeans, Kicks, Jack Purcells</t>
+  </si>
+  <si>
+    <t>Bike Rack, Inner Tube, Pumps</t>
   </si>
 </sst>
 </file>
@@ -701,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -756,59 +747,59 @@
         <v>73</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="18" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="23" t="s">
+      <c r="B10" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="20" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="A13" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>76</v>
-      </c>
+      <c r="B15"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="14" t="s">
@@ -820,28 +811,28 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B18" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="2" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>44</v>
@@ -852,15 +843,15 @@
         <v>68</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -876,14 +867,6 @@
         <v>61</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="21" t="s">
         <v>44</v>
       </c>
     </row>
@@ -894,6 +877,169 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3">
+      <c r="A3" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="16">
+        <v>40931</v>
+      </c>
+      <c r="B4" s="16">
+        <v>40944</v>
+      </c>
+      <c r="C4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="16">
+        <v>40945</v>
+      </c>
+      <c r="B5" s="16">
+        <v>40958</v>
+      </c>
+      <c r="C5">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="16">
+        <v>40959</v>
+      </c>
+      <c r="B6" s="16">
+        <v>40972</v>
+      </c>
+      <c r="C6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="16">
+        <v>40973</v>
+      </c>
+      <c r="B7" s="16">
+        <v>40986</v>
+      </c>
+      <c r="C7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="16">
+        <v>40987</v>
+      </c>
+      <c r="B8" s="16">
+        <v>41000</v>
+      </c>
+      <c r="C8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="16">
+        <v>41001</v>
+      </c>
+      <c r="B9" s="16">
+        <v>41014</v>
+      </c>
+      <c r="C9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="16">
+        <v>41015</v>
+      </c>
+      <c r="B10" s="16">
+        <v>41028</v>
+      </c>
+      <c r="C10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="16">
+        <v>41029</v>
+      </c>
+      <c r="B11" s="16">
+        <v>41042</v>
+      </c>
+      <c r="C11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="16">
+        <v>41043</v>
+      </c>
+      <c r="B12" s="16">
+        <v>41056</v>
+      </c>
+      <c r="C12">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="16">
+        <v>41057</v>
+      </c>
+      <c r="B13" s="16">
+        <v>41070</v>
+      </c>
+      <c r="C13">
+        <v>74.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="16">
+        <v>41071</v>
+      </c>
+      <c r="B14" s="16">
+        <v>41084</v>
+      </c>
+      <c r="C14">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="16">
+        <v>41085</v>
+      </c>
+      <c r="B15" s="16">
+        <v>41098</v>
+      </c>
+      <c r="C15">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -973,7 +1119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A10"/>
   <sheetViews>
@@ -1037,12 +1183,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1092,12 +1238,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A9" sqref="A9:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1137,43 +1283,43 @@
         <v>21</v>
       </c>
     </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="2" t="s">
-        <v>43</v>
+      <c r="A10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>41</v>
+      <c r="A11" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="4" t="s">
-        <v>2</v>
+      <c r="A14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1182,7 +1328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A9"/>
   <sheetViews>
@@ -1239,167 +1385,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:3">
-      <c r="A3" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="16">
-        <v>40931</v>
-      </c>
-      <c r="B4" s="16">
-        <v>40944</v>
-      </c>
-      <c r="C4">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="16">
-        <v>40945</v>
-      </c>
-      <c r="B5" s="16">
-        <v>40958</v>
-      </c>
-      <c r="C5">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="16">
-        <v>40959</v>
-      </c>
-      <c r="B6" s="16">
-        <v>40972</v>
-      </c>
-      <c r="C6">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="16">
-        <v>40973</v>
-      </c>
-      <c r="B7" s="16">
-        <v>40986</v>
-      </c>
-      <c r="C7">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="16">
-        <v>40987</v>
-      </c>
-      <c r="B8" s="16">
-        <v>41000</v>
-      </c>
-      <c r="C8">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="16">
-        <v>41001</v>
-      </c>
-      <c r="B9" s="16">
-        <v>41014</v>
-      </c>
-      <c r="C9">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="16">
-        <v>41015</v>
-      </c>
-      <c r="B10" s="16">
-        <v>41028</v>
-      </c>
-      <c r="C10">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="16">
-        <v>41029</v>
-      </c>
-      <c r="B11" s="16">
-        <v>41042</v>
-      </c>
-      <c r="C11">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="16">
-        <v>41043</v>
-      </c>
-      <c r="B12" s="16">
-        <v>41056</v>
-      </c>
-      <c r="C12">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="16">
-        <v>41057</v>
-      </c>
-      <c r="B13" s="16">
-        <v>41070</v>
-      </c>
-      <c r="C13">
-        <v>74.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="16">
-        <v>41071</v>
-      </c>
-      <c r="B14" s="16">
-        <v>41084</v>
-      </c>
-      <c r="C14">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="16">
-        <v>41085</v>
-      </c>
-      <c r="B15" s="16">
-        <v>41098</v>
-      </c>
-      <c r="C15">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Security Attribute now executing; de-coupled Registration of critical functionalities.
</commit_message>
<xml_diff>
--- a/Dev Notes/Master Backlog.xlsx
+++ b/Dev Notes/Master Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6885" tabRatio="829" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6885" tabRatio="829"/>
   </bookViews>
   <sheets>
     <sheet name="Generic Backlog" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Summer 2012?</t>
   </si>
   <si>
-    <t>Goto the Doctor and get checked up</t>
-  </si>
-  <si>
     <t>New Honda Problem List</t>
   </si>
   <si>
@@ -256,10 +253,10 @@
     <t>Buy Resharper</t>
   </si>
   <si>
-    <t>T-Shirts, Jeans, Kicks, Jack Purcells</t>
-  </si>
-  <si>
-    <t>Bike Rack, Inner Tube, Pumps</t>
+    <t>Goto the Doctor and get checked up + Get my shoulder checked</t>
+  </si>
+  <si>
+    <t>T-Shirts (get them!), Jeans, Kicks, Jack Purcells</t>
   </si>
 </sst>
 </file>
@@ -692,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -722,7 +719,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>0</v>
@@ -736,7 +733,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>0</v>
@@ -744,7 +741,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>0</v>
@@ -752,7 +749,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>0</v>
@@ -760,7 +757,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>0</v>
@@ -768,7 +765,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>44</v>
@@ -776,7 +773,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>44</v>
@@ -784,7 +781,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>44</v>
@@ -792,7 +789,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -802,24 +799,24 @@
       <c r="B15"/>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>44</v>
@@ -827,46 +824,38 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>44</v>
+        <v>67</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>75</v>
+        <v>78</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>0</v>
+      <c r="A23" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="21" t="s">
+      <c r="A24" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="21" t="s">
         <v>44</v>
       </c>
     </row>
@@ -880,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -893,13 +882,13 @@
   <sheetData>
     <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1060,7 +1049,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>17</v>
@@ -1095,7 +1084,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1134,47 +1123,47 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
       <c r="A1" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete namespace overhaul for brevity.
</commit_message>
<xml_diff>
--- a/Dev Notes/Master Backlog.xlsx
+++ b/Dev Notes/Master Backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -253,10 +253,19 @@
     <t>Buy Resharper</t>
   </si>
   <si>
-    <t>Goto the Doctor and get checked up + Get my shoulder checked</t>
-  </si>
-  <si>
     <t>T-Shirts (get them!), Jeans, Kicks, Jack Purcells</t>
+  </si>
+  <si>
+    <t>Goto the Doctor and get checked up</t>
+  </si>
+  <si>
+    <t>Bank of America Maintenance Fees</t>
+  </si>
+  <si>
+    <t>Cancel LogMeIn.com</t>
+  </si>
+  <si>
+    <t>Get MRI Images from Kachar</t>
   </si>
 </sst>
 </file>
@@ -689,16 +698,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="72.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="62.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
   </cols>
@@ -800,62 +809,86 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="18" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B19" s="14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="20" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B20" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="18" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B24" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="19" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="14" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B26" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="20" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B27" s="21" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More AggService and AggRepo Integration and Unit Tests
</commit_message>
<xml_diff>
--- a/Dev Notes/Master Backlog.xlsx
+++ b/Dev Notes/Master Backlog.xlsx
@@ -8,10 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="Generic Backlog" sheetId="2" r:id="rId1"/>
-    <sheet name="SCIGON Payroll Summary" sheetId="15" r:id="rId2"/>
-    <sheet name="Try, Do, Explore" sheetId="8" r:id="rId3"/>
-    <sheet name="New Honda Problems" sheetId="14" r:id="rId4"/>
-    <sheet name="Stuff To Buy" sheetId="6" r:id="rId5"/>
+    <sheet name="Shopping List" sheetId="6" r:id="rId2"/>
+    <sheet name="SCIGON Payroll Summary" sheetId="15" r:id="rId3"/>
+    <sheet name="Try, Do, Explore" sheetId="8" r:id="rId4"/>
+    <sheet name="New Honda Problems" sheetId="14" r:id="rId5"/>
     <sheet name="Services, Markets &amp; Ideas" sheetId="13" r:id="rId6"/>
     <sheet name="Hosts" sheetId="9" r:id="rId7"/>
   </sheets>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -43,12 +43,6 @@
     <t>Brown Jacket (LL Bean?)</t>
   </si>
   <si>
-    <t>Personal Gear</t>
-  </si>
-  <si>
-    <t>Custom Fitted White Shirts</t>
-  </si>
-  <si>
     <t>Try, Do, Explore</t>
   </si>
   <si>
@@ -91,15 +85,9 @@
     <t>Social Assassin / Game</t>
   </si>
   <si>
-    <t>Jack Purcell</t>
-  </si>
-  <si>
     <t>Born Bolt</t>
   </si>
   <si>
-    <t>Stuff To Buy</t>
-  </si>
-  <si>
     <t>Shared Hosting =&gt; http://discountasp.net</t>
   </si>
   <si>
@@ -211,21 +199,12 @@
     <t>House Hunting Backlog</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Storage Architecture for Media</t>
   </si>
   <si>
-    <t>Configure Automatic Backups</t>
-  </si>
-  <si>
     <t>Find Invoicing Software</t>
   </si>
   <si>
-    <t>Bike Handlebars</t>
-  </si>
-  <si>
     <t>Pleiades (MVC + C# + Git + JavaScript + Azure)</t>
   </si>
   <si>
@@ -238,34 +217,49 @@
     <t>Start Date</t>
   </si>
   <si>
-    <t>De-commission Big Blue</t>
-  </si>
-  <si>
-    <t>Call Tax Accountants</t>
-  </si>
-  <si>
-    <t>CALL GUY BACK</t>
-  </si>
-  <si>
     <t>Buy Student Edition Photoshop</t>
   </si>
   <si>
     <t>Buy Resharper</t>
   </si>
   <si>
-    <t>T-Shirts (get them!), Jeans, Kicks, Jack Purcells</t>
-  </si>
-  <si>
     <t>Goto the Doctor and get checked up</t>
   </si>
   <si>
     <t>Bank of America Maintenance Fees</t>
   </si>
   <si>
-    <t>Cancel LogMeIn.com</t>
-  </si>
-  <si>
     <t>Get MRI Images from Kachar</t>
+  </si>
+  <si>
+    <t>LOL</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Kicks, Jack Purcells</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>Music?</t>
+  </si>
+  <si>
+    <t>Shopping List</t>
+  </si>
+  <si>
+    <t>CD Storage</t>
+  </si>
+  <si>
+    <t>Tax Accountants on SATURDAY 9/8</t>
+  </si>
+  <si>
+    <t>T-Shirts (get them!), Jeans, Kicks</t>
+  </si>
+  <si>
+    <t>Configure Automatic Backups - why Dropbox?  What's that other?</t>
   </si>
 </sst>
 </file>
@@ -698,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -722,13 +716,13 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>0</v>
@@ -742,7 +736,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="18" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>0</v>
@@ -750,146 +744,93 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="18" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="18" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15"/>
-    </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>44</v>
+      <c r="A16" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="18" t="s">
+      <c r="A17" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="14" t="s">
+      <c r="B20" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>44</v>
-      </c>
-    </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
+      <c r="A21" s="14" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>44</v>
+      <c r="B21" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -900,10 +841,103 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.25">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -915,13 +949,13 @@
   <sheetData>
     <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1061,12 +1095,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1075,65 +1109,77 @@
     <col min="2" max="2" width="15.140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25">
+    <row r="1" spans="1:3" ht="23.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="B5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="B7" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
       <c r="B9" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1141,122 +1187,72 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
       <c r="A1" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="23.25">
-      <c r="A1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1277,42 +1273,42 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
       <c r="A1" s="12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:1">
@@ -1332,17 +1328,17 @@
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1365,42 +1361,42 @@
   <sheetData>
     <row r="1" spans="1:1" ht="23.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>